<commit_message>
Code changes to My Vehicles and Dashboard modules
Code changes to My Vehicles and Dashboard modules
</commit_message>
<xml_diff>
--- a/MyMojioWebsite/src/com/mojio/xls/ClaimMojio.xlsx
+++ b/MyMojioWebsite/src/com/mojio/xls/ClaimMojio.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="753" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="753" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="101">
   <si>
     <t>TCID</t>
   </si>
@@ -135,15 +135,18 @@
     <t>Write the password</t>
   </si>
   <si>
-    <t>writeInInputByXpath</t>
-  </si>
-  <si>
-    <t>signInPasswordXpath</t>
+    <t>signInPasswordId</t>
   </si>
   <si>
     <t>col|Sign_In_Password</t>
   </si>
   <si>
+    <t>FAIL Unable to write Error communicating with the remote browser. It may have died.
+Build info: version: '2.42.2', revision: '6a6995d', time: '2014-06-03 17:42:30'
+System info: host: 'optimus-88', ip: '172.16.0.104', os.name: 'Windows 7', os.arch: 'x86', os.version: '6.1', java.version: '1.7.0_67'
+Driver info: driver.version: RemoteWebDriver</t>
+  </si>
+  <si>
     <t>TS006</t>
   </si>
   <si>
@@ -156,6 +159,12 @@
     <t>SubmitXpath</t>
   </si>
   <si>
+    <t>FAIL -- Not able to click on ButtonError communicating with the remote browser. It may have died.
+Build info: version: '2.42.2', revision: '6a6995d', time: '2014-06-03 17:42:30'
+System info: host: 'optimus-88', ip: '172.16.0.104', os.name: 'Windows 7', os.arch: 'x86', os.version: '6.1', java.version: '1.7.0_67'
+Driver info: driver.version: RemoteWebDriver</t>
+  </si>
+  <si>
     <t>TS007</t>
   </si>
   <si>
@@ -165,6 +174,15 @@
     <t>col|Dashboard_Page</t>
   </si>
   <si>
+    <t>Error communicating with the remote browser. It may have died.
+Build info: version: '2.42.2', revision: '6a6995d', time: '2014-06-03 17:42:30'
+System info: host: 'optimus-88', ip: '172.16.0.104', os.name: 'Windows 7', os.arch: 'x86', os.version: '6.1', java.version: '1.7.0_67'
+Driver info: driver.version: RemoteWebDriver</t>
+  </si>
+  <si>
+    <t>FAIL -- Not able to navigate</t>
+  </si>
+  <si>
     <t>Click on My Account</t>
   </si>
   <si>
@@ -189,6 +207,9 @@
     <t>claimMojioUrl</t>
   </si>
   <si>
+    <t>FAIL Not able get the URL</t>
+  </si>
+  <si>
     <t>Verify the Claim Mojio page text</t>
   </si>
   <si>
@@ -313,56 +334,6 @@
   </si>
   <si>
     <t>FAIL</t>
-  </si>
-  <si>
-    <t>FAIL Unable to write Unable to locate element: {"method":"id","selector":"EmailOrUserName"}
-Command duration or timeout: 20.10 seconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: '2.42.2', revision: '6a6995d', time: '2014-06-03 17:42:30'
-System info: host: 'OPTIMUS-89', ip: '10.80.6.152', os.name: 'Windows 7', os.arch: 'amd64', os.version: '6.1', java.version: '1.8.0_11'
-Driver info: org.openqa.selenium.firefox.FirefoxDriver
-Capabilities [{applicationCacheEnabled=true, rotatable=false, handlesAlerts=true, databaseEnabled=true, version=31.0, platform=XP, nativeEvents=false, acceptSslCerts=true, webStorageEnabled=true, locationContextEnabled=true, browserName=firefox, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
-Session ID: 7e8c6245-a5bd-41fc-b32c-ad03de2a7a5c</t>
-  </si>
-  <si>
-    <t>FAIL Unable to write Unable to locate element: {"method":"xpath","selector":"html/body/div[7]/div/div[2]/div[1]/div/fieldset/form[1]/div[2]/div/input"}
-Command duration or timeout: 20.06 seconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: '2.42.2', revision: '6a6995d', time: '2014-06-03 17:42:30'
-System info: host: 'OPTIMUS-89', ip: '10.80.6.152', os.name: 'Windows 7', os.arch: 'amd64', os.version: '6.1', java.version: '1.8.0_11'
-Driver info: org.openqa.selenium.firefox.FirefoxDriver
-Capabilities [{applicationCacheEnabled=true, rotatable=false, handlesAlerts=true, databaseEnabled=true, version=31.0, platform=XP, nativeEvents=false, acceptSslCerts=true, webStorageEnabled=true, locationContextEnabled=true, browserName=firefox, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
-Session ID: 7e8c6245-a5bd-41fc-b32c-ad03de2a7a5c</t>
-  </si>
-  <si>
-    <t>FAIL -- Not able to click on ButtonUnable to locate element: {"method":"id","selector":"myaccount-menu"}
-Command duration or timeout: 20.01 seconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: '2.42.2', revision: '6a6995d', time: '2014-06-03 17:42:30'
-System info: host: 'OPTIMUS-89', ip: '192.168.1.231', os.name: 'Windows 7', os.arch: 'amd64', os.version: '6.1', java.version: '1.8.0_11'
-Driver info: org.openqa.selenium.firefox.FirefoxDriver
-Capabilities [{applicationCacheEnabled=true, rotatable=false, handlesAlerts=true, databaseEnabled=true, version=31.0, platform=XP, nativeEvents=false, acceptSslCerts=true, webStorageEnabled=true, locationContextEnabled=true, browserName=firefox, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
-Session ID: df67f2e1-06d2-42b0-8e2a-ae5fdfa2c46d</t>
-  </si>
-  <si>
-    <t>FAIL -- Not able to click on ButtonUnable to locate element: {"method":"xpath","selector":"//li[@id='claim-mojio-link']/a"}
-Command duration or timeout: 20.03 seconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: '2.42.2', revision: '6a6995d', time: '2014-06-03 17:42:30'
-System info: host: 'OPTIMUS-89', ip: '192.168.1.231', os.name: 'Windows 7', os.arch: 'amd64', os.version: '6.1', java.version: '1.8.0_11'
-Driver info: org.openqa.selenium.firefox.FirefoxDriver
-Capabilities [{applicationCacheEnabled=true, rotatable=false, handlesAlerts=true, databaseEnabled=true, version=31.0, platform=XP, nativeEvents=false, acceptSslCerts=true, webStorageEnabled=true, locationContextEnabled=true, browserName=firefox, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
-Session ID: df67f2e1-06d2-42b0-8e2a-ae5fdfa2c46d</t>
-  </si>
-  <si>
-    <t>FAIL -- Not able to click on ButtonUnable to locate element: {"method":"id","selector":"submit-btn"}
-Command duration or timeout: 20.10 seconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: '2.42.2', revision: '6a6995d', time: '2014-06-03 17:42:30'
-System info: host: 'OPTIMUS-89', ip: '192.168.1.231', os.name: 'Windows 7', os.arch: 'amd64', os.version: '6.1', java.version: '1.8.0_11'
-Driver info: org.openqa.selenium.firefox.FirefoxDriver
-Capabilities [{applicationCacheEnabled=true, rotatable=false, handlesAlerts=true, databaseEnabled=true, version=31.0, platform=XP, nativeEvents=false, acceptSslCerts=true, webStorageEnabled=true, locationContextEnabled=true, browserName=firefox, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
-Session ID: df67f2e1-06d2-42b0-8e2a-ae5fdfa2c46d</t>
   </si>
 </sst>
 </file>
@@ -482,7 +453,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -509,6 +480,10 @@
     </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="6" fontId="0" numFmtId="164" xfId="0">
@@ -618,8 +593,8 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D5" activeCellId="0" pane="topLeft" sqref="D5"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A38" activeCellId="0" pane="topLeft" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -692,7 +667,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -713,8 +688,8 @@
   </sheetPr>
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H1" activeCellId="0" pane="topLeft" sqref="H1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E6" activeCellId="0" pane="topLeft" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -857,16 +832,16 @@
         <v>36</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="G6" s="5"/>
-      <c r="H6" s="0" t="s">
+      <c r="H6" s="7" t="s">
         <v>21</v>
       </c>
     </row>
@@ -888,7 +863,7 @@
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="0" t="s">
+      <c r="H7" s="7" t="s">
         <v>21</v>
       </c>
     </row>
@@ -897,261 +872,261 @@
         <v>3</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>28</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G8" s="5"/>
-      <c r="H8" s="0" t="s">
+      <c r="H8" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="9">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7" t="s">
+      <c r="E9" s="8"/>
+      <c r="F9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="7"/>
+      <c r="G9" s="8"/>
       <c r="H9" s="0" t="s">
         <v>21</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="10">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="0" t="s">
+      <c r="C10" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="11">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="7" t="s">
+      <c r="C11" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="0" t="s">
+      <c r="E11" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="12">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
+      <c r="C12" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
       <c r="H12" s="0" t="s">
         <v>21</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="13">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="C13" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="0" t="s">
+      <c r="E13" s="8"/>
+      <c r="F13" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="8"/>
+      <c r="H13" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="14">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8" t="s">
+      <c r="E14" s="9"/>
+      <c r="F14" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="8"/>
+      <c r="G14" s="9"/>
       <c r="H14" t="s">
         <v>21</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="15">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
+      <c r="C15" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
       <c r="H15" t="s">
         <v>21</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="16">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="8" t="s">
+      <c r="C16" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
+      <c r="E16" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
       <c r="H16" t="s">
         <v>21</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="17">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
+      <c r="C17" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
       <c r="H17" t="s">
         <v>21</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="18">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
+      <c r="C18" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
       <c r="H18" t="s">
         <v>21</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="19">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" s="8" t="s">
+      <c r="C19" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="G19" s="8"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G19" s="9"/>
       <c r="H19" t="s">
         <v>21</v>
       </c>
@@ -1183,13 +1158,13 @@
         <v>22</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
@@ -1202,16 +1177,16 @@
         <v>26</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>42</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F22" s="5"/>
-      <c r="G22" s="9"/>
+      <c r="G22" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="23">
       <c r="A23" s="5" t="s">
@@ -1220,17 +1195,17 @@
       <c r="B23" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>57</v>
+      <c r="C23" s="10" t="s">
+        <v>61</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
+        <v>63</v>
+      </c>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="24">
       <c r="A24" s="5" t="s">
@@ -1239,17 +1214,17 @@
       <c r="B24" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>64</v>
+      <c r="C24" s="10" t="s">
+        <v>68</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
+        <v>51</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="25">
       <c r="A25" s="5" t="s">
@@ -1258,263 +1233,245 @@
       <c r="B25" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>66</v>
+      <c r="C25" s="10" t="s">
+        <v>70</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>28</v>
       </c>
       <c r="E25" s="5"/>
-      <c r="F25" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="G25" s="9"/>
+      <c r="F25" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="G25" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="26">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7" t="s">
+      <c r="E26" s="8"/>
+      <c r="F26" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G26" s="11"/>
+      <c r="G26" s="12"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="27">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F27" s="7"/>
-      <c r="G27" s="11"/>
+      <c r="C27" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="8"/>
+      <c r="G27" s="12"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="28">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F28" s="8"/>
+      <c r="G28" s="12"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="29">
+      <c r="A29" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G29" s="12"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="30">
+      <c r="A30" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="31">
+      <c r="A31" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="8"/>
+      <c r="F31" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G31" s="12"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="32">
+      <c r="A32" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G32" s="9"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="33">
+      <c r="A33" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D33" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="34">
+      <c r="A34" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E34" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="35">
+      <c r="A35" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F28" s="7"/>
-      <c r="G28" s="11"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="29">
-      <c r="A29" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F29" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="G29" s="11"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="30">
-      <c r="A30" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B30" s="7" t="s">
+      <c r="E35" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="36">
+      <c r="A36" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="31">
-      <c r="A31" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" s="7" t="s">
+      <c r="C36" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="G36" s="9"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="37">
+      <c r="A37" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="G31" s="11"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="32">
-      <c r="A32" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G32" s="8"/>
-      <c r="H32" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="33">
-      <c r="A33" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="34">
-      <c r="A34" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="35">
-      <c r="A35" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="36">
-      <c r="A36" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="G36" s="8"/>
-      <c r="H36" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="37">
-      <c r="A37" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="0" t="s">
-        <v>21</v>
-      </c>
+      <c r="C37" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1550,16 +1507,16 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>2</v>
@@ -1567,16 +1524,16 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>4</v>
@@ -1613,15 +1570,15 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.05" outlineLevel="0" r="2">
-      <c r="A2" s="13" t="s">
-        <v>85</v>
+      <c r="A2" s="14" t="s">
+        <v>89</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>4</v>
@@ -1658,15 +1615,15 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.05" outlineLevel="0" r="2">
-      <c r="A2" s="13" t="s">
-        <v>87</v>
+      <c r="A2" s="14" t="s">
+        <v>91</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>4</v>
@@ -1703,15 +1660,15 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.05" outlineLevel="0" r="2">
-      <c r="A2" s="13" t="s">
-        <v>89</v>
+      <c r="A2" s="14" t="s">
+        <v>93</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>4</v>
@@ -1749,10 +1706,10 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>2</v>
@@ -1760,10 +1717,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.05" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>93</v>
+        <v>96</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>97</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>4</v>
@@ -1800,15 +1757,15 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.05" outlineLevel="0" r="2">
-      <c r="A2" s="13" t="s">
-        <v>95</v>
+      <c r="A2" s="14" t="s">
+        <v>99</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>4</v>

</xml_diff>